<commit_message>
Adicionado imgs,arvore com 3 cat,alteracao em decisionTreeClassifier
</commit_message>
<xml_diff>
--- a/interin_data/database_validation.xlsx
+++ b/interin_data/database_validation.xlsx
@@ -437,77 +437,77 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>discretization_sqft_lot15</t>
+          <t>disc_sqft_lot15</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>discretization_sqft_living15</t>
+          <t>disc_sqft_living15</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>discretization_yr_renovated</t>
+          <t>disc_yr_renovated</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>discretization_yr_built</t>
+          <t>disc_yr_built</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>discretization_sqft_basement</t>
+          <t>disc_sqft_basement</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>discretization_sqft_above</t>
+          <t>disc_sqft_above</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>discretization_grade</t>
+          <t>disc_grade</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>discretization_condition</t>
+          <t>disc_condition</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>discretization_view</t>
+          <t>disc_view</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>discretization_floors</t>
+          <t>disc_floors</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>discretization_bedrooms</t>
+          <t>disc_bedrooms</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>discretization_bathrooms</t>
+          <t>disc_bathrooms</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>discretization_sqft_lot</t>
+          <t>disc_sqft_lot</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>discretization_sqft_living</t>
+          <t>disc_sqft_living</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>discretization_lat_long</t>
+          <t>disc_lat_long</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -518,7 +518,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -530,16 +530,16 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -554,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -580,16 +580,16 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -604,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
         <v>1</v>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -627,19 +627,19 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -686,10 +686,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -704,13 +704,13 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
         <v>1</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -727,19 +727,19 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -754,7 +754,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
         <v>1</v>
@@ -768,10 +768,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -780,16 +780,16 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -798,30 +798,30 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -830,16 +830,16 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -848,27 +848,27 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -877,19 +877,19 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -904,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
         <v>1</v>
@@ -913,12 +913,12 @@
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -930,37 +930,37 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
         <v>1</v>
       </c>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
         <v>1</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -977,19 +977,19 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>

</xml_diff>